<commit_message>
make some changes in error handle function
</commit_message>
<xml_diff>
--- a/db_structure_formatted.xlsx
+++ b/db_structure_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\collegework\event-management-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB23C19-7D10-46C0-A239-72D9809A251A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B163290-129B-4510-BEE7-554C66064751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="119">
   <si>
     <t>File name</t>
   </si>
@@ -375,6 +375,27 @@
   </si>
   <si>
     <t>OrganiserId field</t>
+  </si>
+  <si>
+    <t>paymentid</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Payment Id field</t>
+  </si>
+  <si>
+    <t>razorpaySignature</t>
+  </si>
+  <si>
+    <t>Razorpay Signature field</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Amount field</t>
   </si>
 </sst>
 </file>
@@ -768,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:F81"/>
+  <dimension ref="A4:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="146" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="154" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,13 +1262,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="2">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>15</v>
@@ -1256,12 +1277,12 @@
         <v>10</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>13</v>
@@ -1276,18 +1297,18 @@
         <v>10</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C34" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>15</v>
@@ -1296,18 +1317,18 @@
         <v>10</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="2">
-        <v>100</v>
+      <c r="C35" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>15</v>
@@ -1316,15 +1337,15 @@
         <v>10</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>15</v>
@@ -1336,15 +1357,15 @@
         <v>10</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>15</v>
@@ -1353,15 +1374,15 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>7</v>
@@ -1376,12 +1397,12 @@
         <v>88</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>7</v>
@@ -1396,72 +1417,72 @@
         <v>88</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="2">
         <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="2">
-        <v>15</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="2" t="s">
         <v>81</v>
       </c>
     </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>5</v>
+      <c r="A44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>7</v>
@@ -1470,18 +1491,18 @@
         <v>15</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>7</v>
@@ -1496,52 +1517,52 @@
         <v>10</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="2" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>5</v>
+      <c r="A54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>7</v>
@@ -1550,44 +1571,44 @@
         <v>15</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C56" s="2">
+        <v>30</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="2">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>15</v>
@@ -1596,72 +1617,72 @@
         <v>10</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="2" t="s">
         <v>109</v>
       </c>
     </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>5</v>
+      <c r="A65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>7</v>
@@ -1670,18 +1691,18 @@
         <v>15</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>7</v>
@@ -1696,35 +1717,35 @@
         <v>10</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>15</v>
@@ -1736,146 +1757,186 @@
         <v>10</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="B72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F70" s="2" t="s">
+      <c r="E72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F73" s="1" t="s">
+      <c r="E75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D74" s="2" t="s">
+      <c r="B76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F74" s="2" t="s">
+      <c r="E76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="2">
+      <c r="B77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="2">
         <v>20</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F75" s="2" t="s">
+      <c r="D77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F79" s="1" t="s">
+      <c r="E81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="2" t="s">
+      <c r="E82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" s="2">
+      <c r="B83" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="2">
         <v>20</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="D83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>